<commit_message>
Update Work Tracking/Time Sheet.xlsx
</commit_message>
<xml_diff>
--- a/Work Tracking/Time Sheet.xlsx
+++ b/Work Tracking/Time Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Desktop/Summer-2019/scrabble/Work Hours/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Desktop/Summer-2019/scrabble/Work Tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13B92CAD-8ABA-3643-8404-BF22716EBAD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4F1ED72-FB8E-6C43-8DE3-A68348F7DDD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16600" xr2:uid="{90E5CAA6-A1ED-BB4C-A20E-228CFC255461}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>DATE</t>
   </si>
@@ -36,9 +36,6 @@
     <t>OUT</t>
   </si>
   <si>
-    <t>Out</t>
-  </si>
-  <si>
     <t>MONDAY</t>
   </si>
   <si>
@@ -64,14 +61,31 @@
   </si>
   <si>
     <t>HOURS WORKED</t>
+  </si>
+  <si>
+    <t>TOTAL HOURS:</t>
+  </si>
+  <si>
+    <t>IN2</t>
+  </si>
+  <si>
+    <t>OUT2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -95,21 +109,366 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -120,6 +479,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{302CF30A-29A8-504D-BB11-E182EF979F5F}" name="Table1" displayName="Table1" ref="A1:G15" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:G15" xr:uid="{7909C85F-5AC1-1C41-A0DA-FEFDDD3083B4}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{AC16E83B-DFE2-A24F-BCA4-3256B6AA2E2E}" name="DAY" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F1A89DD6-FD0F-B749-9D77-151E6C6CBCFA}" name="DATE" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{20BB48E1-AA0D-3E47-AD77-73131EC31B2F}" name="IN" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{38AEDD78-D8C3-2748-81FB-F61358B2711C}" name="OUT" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E5EF4C67-3789-FD49-9CB0-10736833C336}" name="IN2" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{6774D340-ED72-604A-9FD6-EB1645472754}" name="OUT2" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{7FF324A6-96B5-3D41-95AC-571DB53028EA}" name="HOURS WORKED" dataDxfId="1">
+      <calculatedColumnFormula>D2-C2+F2-E2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,316 +799,339 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="B2" s="10">
         <v>43612</v>
       </c>
-      <c r="G2" s="2">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12">
         <f t="shared" ref="G2:G4" si="0">D2-C2+F2-E2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="10">
         <v>43613</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="14">
         <v>0.54166666666666663</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="12">
         <f>D3-C3+F3-E3</f>
         <v>0.16666666666666669</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10">
         <v>43614</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G4" s="2">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12">
         <f t="shared" si="0"/>
         <v>0.29166666666666669</v>
       </c>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10">
         <v>43615</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="14">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="14">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="12">
         <f>D5-C5+F5-E5</f>
         <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="10">
         <v>43616</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="14">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="12">
         <f>D6-C6+F6-E6</f>
         <v>0.16666666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="10">
         <v>43617</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="14">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="14">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="12">
         <f>D7-C7+F7-E7</f>
         <v>0.25000000000000017</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="A8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="10">
         <v>43618</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="14">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="12">
         <f>D8-C8+F8-E8</f>
         <v>0.12500000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10">
         <v>43619</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="14">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="14">
         <v>0.875</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="12">
         <f>D9-C9+F9-E9</f>
         <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="10">
         <v>43620</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G10" s="2">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12">
         <f>D10-C10+F10-E10</f>
         <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="10">
         <v>43621</v>
       </c>
-      <c r="G11" s="2">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12">
         <f>D11-C11+F11-E11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="A12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="10">
         <v>43622</v>
       </c>
-      <c r="G12" s="2">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12">
         <f>D12-C12+F12-E12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="A13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="10">
         <v>43623</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="14">
         <v>0.5</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="14">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="14">
         <v>0.95833333333333337</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="12">
         <f>D13-C13+F13-E13</f>
         <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="A14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10">
         <v>43624</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G14" s="2">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12">
         <f>D14-C14+F14-E14</f>
         <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="A15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="16">
         <v>43625</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G15" s="2">
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19">
         <f>D15-C15+F15-E15</f>
         <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
-      <c r="G16" s="4">
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="F17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="5">
         <f>SUM(G2:G15)</f>
         <v>2.8333333333333335</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
@@ -755,5 +1155,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added function to unpackage and display npz files
</commit_message>
<xml_diff>
--- a/Work Tracking/Time Sheet.xlsx
+++ b/Work Tracking/Time Sheet.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Desktop/Summer-2019/scrabble/Work Tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E722332-2E21-EE47-80B1-28D559EAA19C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87399BFE-949B-2C41-AAD7-506ED9A50E5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="2" xr2:uid="{90E5CAA6-A1ED-BB4C-A20E-228CFC255461}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="3" xr2:uid="{90E5CAA6-A1ED-BB4C-A20E-228CFC255461}"/>
   </bookViews>
   <sheets>
     <sheet name="5 27 - 6 9" sheetId="1" r:id="rId1"/>
     <sheet name="June 10th to 23rd" sheetId="3" r:id="rId2"/>
     <sheet name="June 24th to July 7th " sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="July 8th to 21st" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet2 (2)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="17">
   <si>
     <t>DATE</t>
   </si>
@@ -264,7 +266,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="55">
     <dxf>
       <numFmt numFmtId="25" formatCode="h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -723,76 +725,74 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -943,74 +943,76 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1078,30 +1080,30 @@
     <dxf>
       <border>
         <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
@@ -1139,6 +1141,224 @@
         </horizontal>
       </border>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1153,16 +1373,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{302CF30A-29A8-504D-BB11-E182EF979F5F}" name="Table1" displayName="Table1" ref="A1:G15" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{302CF30A-29A8-504D-BB11-E182EF979F5F}" name="Table1" displayName="Table1" ref="A1:G15" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="A1:G15" xr:uid="{7909C85F-5AC1-1C41-A0DA-FEFDDD3083B4}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AC16E83B-DFE2-A24F-BCA4-3256B6AA2E2E}" name="DAY" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{F1A89DD6-FD0F-B749-9D77-151E6C6CBCFA}" name="DATE" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{20BB48E1-AA0D-3E47-AD77-73131EC31B2F}" name="IN" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{38AEDD78-D8C3-2748-81FB-F61358B2711C}" name="OUT" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{E5EF4C67-3789-FD49-9CB0-10736833C336}" name="IN2" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{6774D340-ED72-604A-9FD6-EB1645472754}" name="OUT2" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{7FF324A6-96B5-3D41-95AC-571DB53028EA}" name="HOURS WORKED" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{AC16E83B-DFE2-A24F-BCA4-3256B6AA2E2E}" name="DAY" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{F1A89DD6-FD0F-B749-9D77-151E6C6CBCFA}" name="DATE" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{20BB48E1-AA0D-3E47-AD77-73131EC31B2F}" name="IN" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{38AEDD78-D8C3-2748-81FB-F61358B2711C}" name="OUT" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{E5EF4C67-3789-FD49-9CB0-10736833C336}" name="IN2" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{6774D340-ED72-604A-9FD6-EB1645472754}" name="OUT2" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{7FF324A6-96B5-3D41-95AC-571DB53028EA}" name="HOURS WORKED" dataDxfId="44">
       <calculatedColumnFormula>D2-C2+F2-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1171,16 +1391,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BD9BBBAD-0E4B-FF47-BBC9-43199C6A56A5}" name="Table143" displayName="Table143" ref="A1:G15" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BD9BBBAD-0E4B-FF47-BBC9-43199C6A56A5}" name="Table143" displayName="Table143" ref="A1:G15" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
   <autoFilter ref="A1:G15" xr:uid="{BF5537AC-A15A-9049-B514-2CEBE112C09A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9D4C76CD-B24D-4848-BE2C-3A6F250D2AC4}" name="DAY" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{43D19B11-5450-AD40-AADD-65034905CB49}" name="DATE" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{7EAFA47C-1F57-F44B-8C2E-DBAA8AA52FD1}" name="IN" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{A2F973C1-C96E-CF41-A148-CA138690A9E5}" name="OUT" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{6412FA9D-2708-594C-B091-60ABB5838C49}" name="IN2" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{C7C70BB3-5490-754A-B576-09962ABEB833}" name="OUT2" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{C71D6813-9EF5-414C-9561-50ACA8255127}" name="HOURS WORKED" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{9D4C76CD-B24D-4848-BE2C-3A6F250D2AC4}" name="DAY" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{43D19B11-5450-AD40-AADD-65034905CB49}" name="DATE" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{7EAFA47C-1F57-F44B-8C2E-DBAA8AA52FD1}" name="IN" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{A2F973C1-C96E-CF41-A148-CA138690A9E5}" name="OUT" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{6412FA9D-2708-594C-B091-60ABB5838C49}" name="IN2" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{C7C70BB3-5490-754A-B576-09962ABEB833}" name="OUT2" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{C71D6813-9EF5-414C-9561-50ACA8255127}" name="HOURS WORKED" dataDxfId="33">
       <calculatedColumnFormula>D2-C2+F2-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1189,16 +1409,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F08644F1-0DD8-BA4C-AE1D-BD0767F0BADE}" name="Table145" displayName="Table145" ref="A1:G15" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F08644F1-0DD8-BA4C-AE1D-BD0767F0BADE}" name="Table145" displayName="Table145" ref="A1:G15" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A1:G15" xr:uid="{BF5537AC-A15A-9049-B514-2CEBE112C09A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D6012E41-DFC3-8745-B8F7-EBEC6A9FCA7E}" name="DAY" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{94CA8E12-A53A-E94F-8CBC-F9A716BA6A20}" name="DATE" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{AB7038AA-C380-1C4A-9C70-311EF49DCA75}" name="IN" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{7E8F0CF7-9725-B540-BF9B-EBCCB961E37F}" name="OUT" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{F8F7DDDE-3F36-8B45-9EAE-B833212BF6B1}" name="IN2" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{E68D8CE9-8376-F24A-A795-22CA0E5AF0A3}" name="OUT2" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{0C2D20EA-6480-BE44-A7F6-9E85DEDB90F7}" name="HOURS WORKED" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{D6012E41-DFC3-8745-B8F7-EBEC6A9FCA7E}" name="DAY" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{94CA8E12-A53A-E94F-8CBC-F9A716BA6A20}" name="DATE" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{AB7038AA-C380-1C4A-9C70-311EF49DCA75}" name="IN" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{7E8F0CF7-9725-B540-BF9B-EBCCB961E37F}" name="OUT" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{F8F7DDDE-3F36-8B45-9EAE-B833212BF6B1}" name="IN2" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{E68D8CE9-8376-F24A-A795-22CA0E5AF0A3}" name="OUT2" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{0C2D20EA-6480-BE44-A7F6-9E85DEDB90F7}" name="HOURS WORKED" dataDxfId="22">
       <calculatedColumnFormula>D2-C2+F2-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1217,6 +1437,24 @@
     <tableColumn id="5" xr3:uid="{88412330-D8E4-E84D-8E58-13DD26E5E2C9}" name="IN2" dataDxfId="13"/>
     <tableColumn id="6" xr3:uid="{5C6D956C-34D0-CE4B-9B02-376B54AF0868}" name="OUT2" dataDxfId="12"/>
     <tableColumn id="7" xr3:uid="{659D80D8-1F98-1540-ADDF-C5872E7A9CAB}" name="HOURS WORKED" dataDxfId="11">
+      <calculatedColumnFormula>D2-C2+F2-E2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FE70DB98-979E-AB49-A8CD-98FE8BD0F598}" name="Table146" displayName="Table146" ref="A1:G15" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:G15" xr:uid="{BF5537AC-A15A-9049-B514-2CEBE112C09A}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{C51A1474-F9F7-A542-BBAF-EC104927BA22}" name="DAY" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{1EAE3B48-AC3F-1A4D-9E70-24C2D76FF5EB}" name="DATE" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{DA38AC75-7938-924C-A5B7-2EA329D6BB48}" name="IN" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{000CB6BA-745F-F440-AB4C-FD6AB8DA7427}" name="OUT" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{ADA596AA-F0AA-044C-AE80-BE49132FD2B3}" name="IN2" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{8CD2B17E-4C8C-D44E-B12A-1185D5925AA7}" name="OUT2" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{D387DD68-F8FC-CC40-B865-E095A963272D}" name="HOURS WORKED" dataDxfId="0">
       <calculatedColumnFormula>D2-C2+F2-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2252,7 +2490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E104A721-2F43-2345-AB0A-02E0AAC309D4}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" workbookViewId="0">
+    <sheetView zoomScale="149" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2605,6 +2843,309 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266EB692-21B1-BA4D-91A7-4364896ECCDF}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="18">
+        <v>43654</v>
+      </c>
+      <c r="C2" s="14">
+        <v>0.4375</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12">
+        <f t="shared" ref="G2:G4" si="0">D2-C2+F2-E2</f>
+        <v>0.29166666666666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="18">
+        <v>43655</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="12">
+        <f>D3-C3+F3-E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18">
+        <v>43656</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="18">
+        <v>43657</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="12">
+        <f t="shared" ref="G5:G15" si="1">D5-C5+F5-E5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="18">
+        <v>43658</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="18">
+        <v>43659</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="4">
+        <f>SUM(G2:G8)</f>
+        <v>0.29166666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="18">
+        <v>43660</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="18">
+        <v>43661</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="18">
+        <v>43662</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="18">
+        <v>43663</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18">
+        <v>43664</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="18">
+        <v>43665</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="18">
+        <v>43666</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="18">
+        <v>43667</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="4">
+        <f>SUM(G9:G15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="F17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="6">
+        <f>SUM(G2:G15)</f>
+        <v>0.29166666666666663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE157A8-94FF-FB44-BBDB-29F9D57601B0}">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
@@ -2654,7 +3195,7 @@
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="12">
-        <f t="shared" ref="G2:G4" si="0">D2-C2+F2-E2</f>
+        <f t="shared" ref="G2:G15" si="0">D2-C2+F2-E2</f>
         <v>0</v>
       </c>
     </row>
@@ -2703,7 +3244,7 @@
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="12">
-        <f t="shared" ref="G5:G15" si="1">D5-C5+F5-E5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2719,7 +3260,7 @@
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2735,7 +3276,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I7" t="s">
@@ -2758,7 +3299,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2774,7 +3315,7 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2790,7 +3331,7 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2806,7 +3347,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2822,7 +3363,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2838,7 +3379,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2854,7 +3395,7 @@
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2870,7 +3411,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15" t="s">

</xml_diff>